<commit_message>
Add HLE 2017-19 data
</commit_message>
<xml_diff>
--- a/data/HLE.xlsx
+++ b/data/HLE.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11011"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\u442941\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rhiannonbatstone/population_dashboard/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E447B4CF-311F-E04D-86BE-A1D38FCB8366}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060"/>
+    <workbookView xWindow="14760" yWindow="-24000" windowWidth="19000" windowHeight="24000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="HLE" sheetId="11" r:id="rId1"/>
@@ -22,18 +23,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1368" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1698" uniqueCount="88">
   <si>
     <t>Males</t>
   </si>
@@ -289,11 +284,20 @@
   <si>
     <t>Perth and Kinross</t>
   </si>
+  <si>
+    <t>2017-19</t>
+  </si>
+  <si>
+    <t>S12000049</t>
+  </si>
+  <si>
+    <t>S12000050</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -638,25 +642,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H273"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H339"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+    <sheetView tabSelected="1" topLeftCell="A280" workbookViewId="0">
+      <selection activeCell="C228" sqref="C228:C229"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.5703125" customWidth="1"/>
+    <col min="1" max="1" width="8.5" customWidth="1"/>
     <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="28.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="28.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="13.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -682,7 +686,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>20</v>
       </c>
@@ -708,7 +712,7 @@
         <v>70.075847489011693</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -734,7 +738,7 @@
         <v>68.403014556172593</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -760,7 +764,7 @@
         <v>66.848862873161806</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -786,7 +790,7 @@
         <v>65.735395524593699</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>20</v>
       </c>
@@ -812,7 +816,7 @@
         <v>66.120460068017806</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -838,7 +842,7 @@
         <v>64.963558672552494</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -864,7 +868,7 @@
         <v>63.564984304031199</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -890,7 +894,7 @@
         <v>63.010625495473697</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>20</v>
       </c>
@@ -916,7 +920,7 @@
         <v>67.254329149681297</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>5</v>
       </c>
@@ -942,7 +946,7 @@
         <v>70.142273903826293</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>6</v>
       </c>
@@ -968,7 +972,7 @@
         <v>69.122788696727895</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>7</v>
       </c>
@@ -994,7 +998,7 @@
         <v>70.001348312639095</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>20</v>
       </c>
@@ -1020,7 +1024,7 @@
         <v>67.546422990757307</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>5</v>
       </c>
@@ -1046,7 +1050,7 @@
         <v>68.629285415978998</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>6</v>
       </c>
@@ -1072,7 +1076,7 @@
         <v>69.779541975383907</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>7</v>
       </c>
@@ -1098,7 +1102,7 @@
         <v>70.5947681054176</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>20</v>
       </c>
@@ -1124,7 +1128,7 @@
         <v>66.397119999258393</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>5</v>
       </c>
@@ -1150,7 +1154,7 @@
         <v>66.6232265101129</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>6</v>
       </c>
@@ -1176,7 +1180,7 @@
         <v>65.343367553735405</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>7</v>
       </c>
@@ -1202,7 +1206,7 @@
         <v>65.539642766869406</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>20</v>
       </c>
@@ -1228,7 +1232,7 @@
         <v>67.141526410640694</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>5</v>
       </c>
@@ -1254,7 +1258,7 @@
         <v>66.264079868838806</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>6</v>
       </c>
@@ -1280,7 +1284,7 @@
         <v>64.892964103713993</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>7</v>
       </c>
@@ -1306,7 +1310,7 @@
         <v>63.270265469890703</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>20</v>
       </c>
@@ -1332,7 +1336,7 @@
         <v>65.368561980293904</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>5</v>
       </c>
@@ -1358,7 +1362,7 @@
         <v>66.349036946715202</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>6</v>
       </c>
@@ -1384,7 +1388,7 @@
         <v>64.344659428265999</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>7</v>
       </c>
@@ -1410,7 +1414,7 @@
         <v>64.909628892966396</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>20</v>
       </c>
@@ -1436,7 +1440,7 @@
         <v>65.300124927097997</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>5</v>
       </c>
@@ -1462,7 +1466,7 @@
         <v>65.987575950301704</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>6</v>
       </c>
@@ -1488,7 +1492,7 @@
         <v>65.823466832507293</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>7</v>
       </c>
@@ -1514,7 +1518,7 @@
         <v>66.695781091488698</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>20</v>
       </c>
@@ -1540,7 +1544,7 @@
         <v>67.375515060849906</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>5</v>
       </c>
@@ -1566,7 +1570,7 @@
         <v>68.497459776272805</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>6</v>
       </c>
@@ -1592,7 +1596,7 @@
         <v>67.540418392824606</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>7</v>
       </c>
@@ -1618,7 +1622,7 @@
         <v>66.104650434502602</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>20</v>
       </c>
@@ -1644,7 +1648,7 @@
         <v>66.587490875359507</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>5</v>
       </c>
@@ -1670,7 +1674,7 @@
         <v>66.891479477950298</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>6</v>
       </c>
@@ -1696,7 +1700,7 @@
         <v>66.863918858875607</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>7</v>
       </c>
@@ -1722,7 +1726,7 @@
         <v>67.198253968678898</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>20</v>
       </c>
@@ -1748,7 +1752,7 @@
         <v>63.4169634555941</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>5</v>
       </c>
@@ -1774,7 +1778,7 @@
         <v>61.331660847117099</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>6</v>
       </c>
@@ -1800,7 +1804,7 @@
         <v>63.083686809793498</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>7</v>
       </c>
@@ -1826,7 +1830,7 @@
         <v>64.502413702527306</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>20</v>
       </c>
@@ -1852,7 +1856,7 @@
         <v>63.0775739662378</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>5</v>
       </c>
@@ -1878,7 +1882,7 @@
         <v>62.124196355956798</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>6</v>
       </c>
@@ -1904,7 +1908,7 @@
         <v>65.007148032242696</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>7</v>
       </c>
@@ -1930,7 +1934,7 @@
         <v>64.736424752204599</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>20</v>
       </c>
@@ -1956,7 +1960,7 @@
         <v>65.371289640374698</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>5</v>
       </c>
@@ -1982,7 +1986,7 @@
         <v>67.740229835936105</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>6</v>
       </c>
@@ -2008,7 +2012,7 @@
         <v>65.923359188301603</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>7</v>
       </c>
@@ -2034,7 +2038,7 @@
         <v>66.3961972885253</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>20</v>
       </c>
@@ -2060,7 +2064,7 @@
         <v>65.010278668313504</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>5</v>
       </c>
@@ -2086,7 +2090,7 @@
         <v>66.056774818153301</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>6</v>
       </c>
@@ -2112,7 +2116,7 @@
         <v>65.970606517153897</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>7</v>
       </c>
@@ -2138,7 +2142,7 @@
         <v>65.807040685706099</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>20</v>
       </c>
@@ -2164,7 +2168,7 @@
         <v>63.989132056066701</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>5</v>
       </c>
@@ -2190,7 +2194,7 @@
         <v>63.652076380790596</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>6</v>
       </c>
@@ -2216,7 +2220,7 @@
         <v>62.052287411741901</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>7</v>
       </c>
@@ -2242,7 +2246,7 @@
         <v>61.900254687945598</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>20</v>
       </c>
@@ -2268,7 +2272,7 @@
         <v>60.113989500983898</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>5</v>
       </c>
@@ -2294,7 +2298,7 @@
         <v>56.9323580925223</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>6</v>
       </c>
@@ -2320,7 +2324,7 @@
         <v>58.639486221201203</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>7</v>
       </c>
@@ -2346,7 +2350,7 @@
         <v>58.5381699351815</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>20</v>
       </c>
@@ -2372,7 +2376,7 @@
         <v>60.272413096237898</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>5</v>
       </c>
@@ -2398,7 +2402,7 @@
         <v>60.300044855795001</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>6</v>
       </c>
@@ -2424,7 +2428,7 @@
         <v>60.382250436571901</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>7</v>
       </c>
@@ -2450,7 +2454,7 @@
         <v>60.883962134839898</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>20</v>
       </c>
@@ -2476,7 +2480,7 @@
         <v>59.808412393752398</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>5</v>
       </c>
@@ -2502,7 +2506,7 @@
         <v>61.147677102830599</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>6</v>
       </c>
@@ -2528,7 +2532,7 @@
         <v>62.104910752520603</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>7</v>
       </c>
@@ -2554,7 +2558,7 @@
         <v>59.879917170479303</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>20</v>
       </c>
@@ -2580,7 +2584,7 @@
         <v>69.607003838904106</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>5</v>
       </c>
@@ -2606,7 +2610,7 @@
         <v>71.335170529740495</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>6</v>
       </c>
@@ -2632,7 +2636,7 @@
         <v>69.975323106482804</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>7</v>
       </c>
@@ -2658,7 +2662,7 @@
         <v>70.146431754754104</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>20</v>
       </c>
@@ -2684,7 +2688,7 @@
         <v>66.738170669527406</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>5</v>
       </c>
@@ -2710,7 +2714,7 @@
         <v>67.048959998099306</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>6</v>
       </c>
@@ -2736,7 +2740,7 @@
         <v>70.476165749492594</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>7</v>
       </c>
@@ -2762,7 +2766,7 @@
         <v>71.252712956565901</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>20</v>
       </c>
@@ -2788,7 +2792,7 @@
         <v>70.035466784596593</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>5</v>
       </c>
@@ -2814,7 +2818,7 @@
         <v>69.501419944408497</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>6</v>
       </c>
@@ -2840,7 +2844,7 @@
         <v>66.113294170215795</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>7</v>
       </c>
@@ -2866,7 +2870,7 @@
         <v>66.173302712097495</v>
       </c>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>20</v>
       </c>
@@ -2892,7 +2896,7 @@
         <v>65.582637463250407</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>5</v>
       </c>
@@ -2918,7 +2922,7 @@
         <v>68.072887414476696</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>6</v>
       </c>
@@ -2944,7 +2948,7 @@
         <v>67.169819221668405</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>7</v>
       </c>
@@ -2970,7 +2974,7 @@
         <v>67.303721898865206</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>20</v>
       </c>
@@ -2996,7 +3000,7 @@
         <v>68.864339187365701</v>
       </c>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>5</v>
       </c>
@@ -3022,7 +3026,7 @@
         <v>68.693541423056999</v>
       </c>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>6</v>
       </c>
@@ -3048,7 +3052,7 @@
         <v>67.6692985450387</v>
       </c>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>7</v>
       </c>
@@ -3074,7 +3078,7 @@
         <v>68.316584263850103</v>
       </c>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>20</v>
       </c>
@@ -3100,7 +3104,7 @@
         <v>67.583316893324593</v>
       </c>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>5</v>
       </c>
@@ -3126,7 +3130,7 @@
         <v>67.849977583803906</v>
       </c>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>6</v>
       </c>
@@ -3152,7 +3156,7 @@
         <v>68.480788623569794</v>
       </c>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>7</v>
       </c>
@@ -3178,7 +3182,7 @@
         <v>70.653408042768007</v>
       </c>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>20</v>
       </c>
@@ -3204,7 +3208,7 @@
         <v>65.622546901726693</v>
       </c>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>5</v>
       </c>
@@ -3230,7 +3234,7 @@
         <v>65.388282994353901</v>
       </c>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>6</v>
       </c>
@@ -3256,7 +3260,7 @@
         <v>62.865803487504898</v>
       </c>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>7</v>
       </c>
@@ -3282,7 +3286,7 @@
         <v>62.159942762157101</v>
       </c>
     </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>20</v>
       </c>
@@ -3308,7 +3312,7 @@
         <v>63.328158378057402</v>
       </c>
     </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>5</v>
       </c>
@@ -3334,7 +3338,7 @@
         <v>63.007720455626398</v>
       </c>
     </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>6</v>
       </c>
@@ -3360,7 +3364,7 @@
         <v>65.028032514990699</v>
       </c>
     </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>7</v>
       </c>
@@ -3386,7 +3390,7 @@
         <v>63.896157712364797</v>
       </c>
     </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>20</v>
       </c>
@@ -3412,7 +3416,7 @@
         <v>62.561401801110399</v>
       </c>
     </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>5</v>
       </c>
@@ -3438,7 +3442,7 @@
         <v>64.450752171148594</v>
       </c>
     </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>6</v>
       </c>
@@ -3464,7 +3468,7 @@
         <v>64.262121352275898</v>
       </c>
     </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>7</v>
       </c>
@@ -3490,7 +3494,7 @@
         <v>62.343574953703097</v>
       </c>
     </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>20</v>
       </c>
@@ -3516,7 +3520,7 @@
         <v>63.311510978769803</v>
       </c>
     </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>5</v>
       </c>
@@ -3542,7 +3546,7 @@
         <v>63.196481608770199</v>
       </c>
     </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>6</v>
       </c>
@@ -3568,7 +3572,7 @@
         <v>64.170312047051496</v>
       </c>
     </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>7</v>
       </c>
@@ -3594,7 +3598,7 @@
         <v>62.943669525270003</v>
       </c>
     </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>20</v>
       </c>
@@ -3620,7 +3624,7 @@
         <v>59.375683999755502</v>
       </c>
     </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>5</v>
       </c>
@@ -3646,7 +3650,7 @@
         <v>60.987888158749897</v>
       </c>
     </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>6</v>
       </c>
@@ -3672,7 +3676,7 @@
         <v>60.8374714088405</v>
       </c>
     </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>7</v>
       </c>
@@ -3698,7 +3702,7 @@
         <v>60.119250795089101</v>
       </c>
     </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>20</v>
       </c>
@@ -3724,7 +3728,7 @@
         <v>57.688050299555798</v>
       </c>
     </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>5</v>
       </c>
@@ -3750,7 +3754,7 @@
         <v>60.343679445626897</v>
       </c>
     </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>6</v>
       </c>
@@ -3776,7 +3780,7 @@
         <v>58.991422246658097</v>
       </c>
     </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>7</v>
       </c>
@@ -3802,7 +3806,7 @@
         <v>57.717488079886898</v>
       </c>
     </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>20</v>
       </c>
@@ -3828,7 +3832,7 @@
         <v>67.237291165348793</v>
       </c>
     </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>5</v>
       </c>
@@ -3854,7 +3858,7 @@
         <v>65.533405614456399</v>
       </c>
     </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>6</v>
       </c>
@@ -3880,7 +3884,7 @@
         <v>66.170687265992399</v>
       </c>
     </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>7</v>
       </c>
@@ -3906,7 +3910,7 @@
         <v>68.172092797557198</v>
       </c>
     </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>20</v>
       </c>
@@ -3932,7 +3936,7 @@
         <v>66.487942829101598</v>
       </c>
     </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>5</v>
       </c>
@@ -3958,7 +3962,7 @@
         <v>67.207661702045399</v>
       </c>
     </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>6</v>
       </c>
@@ -3984,7 +3988,7 @@
         <v>68.083409352931099</v>
       </c>
     </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>7</v>
       </c>
@@ -4010,7 +4014,7 @@
         <v>66.269087341894405</v>
       </c>
     </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>20</v>
       </c>
@@ -4036,7 +4040,7 @@
         <v>61.568337233271798</v>
       </c>
     </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>5</v>
       </c>
@@ -4062,7 +4066,7 @@
         <v>62.525298585284901</v>
       </c>
     </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>6</v>
       </c>
@@ -4088,7 +4092,7 @@
         <v>61.506756069321199</v>
       </c>
     </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>7</v>
       </c>
@@ -4114,7 +4118,7 @@
         <v>61.763463200717503</v>
       </c>
     </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>20</v>
       </c>
@@ -4140,7 +4144,7 @@
         <v>60.0359085659179</v>
       </c>
     </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>5</v>
       </c>
@@ -4166,7 +4170,7 @@
         <v>61.494875084315602</v>
       </c>
     </row>
-    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>6</v>
       </c>
@@ -4192,7 +4196,7 @@
         <v>62.232559036564297</v>
       </c>
     </row>
-    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>7</v>
       </c>
@@ -4218,7 +4222,7 @@
         <v>61.485421697223302</v>
       </c>
     </row>
-    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>20</v>
       </c>
@@ -4244,7 +4248,7 @@
         <v>63.6300879862115</v>
       </c>
     </row>
-    <row r="139" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>5</v>
       </c>
@@ -4270,7 +4274,7 @@
         <v>65.962695506169297</v>
       </c>
     </row>
-    <row r="140" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>6</v>
       </c>
@@ -4296,7 +4300,7 @@
         <v>66.235687395070897</v>
       </c>
     </row>
-    <row r="141" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>7</v>
       </c>
@@ -4322,7 +4326,7 @@
         <v>65.855821787127198</v>
       </c>
     </row>
-    <row r="142" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>20</v>
       </c>
@@ -4348,7 +4352,7 @@
         <v>64.417106449775005</v>
       </c>
     </row>
-    <row r="143" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>5</v>
       </c>
@@ -4374,7 +4378,7 @@
         <v>64.060317034476597</v>
       </c>
     </row>
-    <row r="144" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>6</v>
       </c>
@@ -4400,7 +4404,7 @@
         <v>63.9201486263321</v>
       </c>
     </row>
-    <row r="145" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>7</v>
       </c>
@@ -4426,7 +4430,7 @@
         <v>63.287975418737503</v>
       </c>
     </row>
-    <row r="146" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>20</v>
       </c>
@@ -4452,7 +4456,7 @@
         <v>67.396505860003302</v>
       </c>
     </row>
-    <row r="147" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>5</v>
       </c>
@@ -4478,7 +4482,7 @@
         <v>68.040258848270796</v>
       </c>
     </row>
-    <row r="148" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>6</v>
       </c>
@@ -4504,7 +4508,7 @@
         <v>66.313387756014706</v>
       </c>
     </row>
-    <row r="149" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>7</v>
       </c>
@@ -4530,7 +4534,7 @@
         <v>64.389917125523496</v>
       </c>
     </row>
-    <row r="150" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>20</v>
       </c>
@@ -4556,7 +4560,7 @@
         <v>68.054432268901905</v>
       </c>
     </row>
-    <row r="151" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>5</v>
       </c>
@@ -4582,7 +4586,7 @@
         <v>67.432823297684394</v>
       </c>
     </row>
-    <row r="152" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>6</v>
       </c>
@@ -4608,7 +4612,7 @@
         <v>66.180904690681501</v>
       </c>
     </row>
-    <row r="153" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
         <v>7</v>
       </c>
@@ -4634,7 +4638,7 @@
         <v>64.163305890158597</v>
       </c>
     </row>
-    <row r="154" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
         <v>20</v>
       </c>
@@ -4660,7 +4664,7 @@
         <v>72.721650158811002</v>
       </c>
     </row>
-    <row r="155" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
         <v>5</v>
       </c>
@@ -4686,7 +4690,7 @@
         <v>69.2204243278711</v>
       </c>
     </row>
-    <row r="156" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
         <v>6</v>
       </c>
@@ -4712,7 +4716,7 @@
         <v>70.488642806143702</v>
       </c>
     </row>
-    <row r="157" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
         <v>7</v>
       </c>
@@ -4738,7 +4742,7 @@
         <v>69.979752848358899</v>
       </c>
     </row>
-    <row r="158" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
         <v>20</v>
       </c>
@@ -4764,7 +4768,7 @@
         <v>69.828442746929895</v>
       </c>
     </row>
-    <row r="159" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
         <v>5</v>
       </c>
@@ -4790,7 +4794,7 @@
         <v>67.810667681566599</v>
       </c>
     </row>
-    <row r="160" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
         <v>6</v>
       </c>
@@ -4816,7 +4820,7 @@
         <v>67.665907815217594</v>
       </c>
     </row>
-    <row r="161" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
         <v>7</v>
       </c>
@@ -4842,7 +4846,7 @@
         <v>68.464766666045506</v>
       </c>
     </row>
-    <row r="162" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
         <v>20</v>
       </c>
@@ -4868,7 +4872,7 @@
         <v>58.501255900437698</v>
       </c>
     </row>
-    <row r="163" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
         <v>5</v>
       </c>
@@ -4894,7 +4898,7 @@
         <v>59.068775658282902</v>
       </c>
     </row>
-    <row r="164" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
         <v>6</v>
       </c>
@@ -4920,7 +4924,7 @@
         <v>59.2110191146826</v>
       </c>
     </row>
-    <row r="165" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
         <v>7</v>
       </c>
@@ -4946,7 +4950,7 @@
         <v>58.181500286692398</v>
       </c>
     </row>
-    <row r="166" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
         <v>20</v>
       </c>
@@ -4972,7 +4976,7 @@
         <v>60.377757818801797</v>
       </c>
     </row>
-    <row r="167" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
         <v>5</v>
       </c>
@@ -4998,7 +5002,7 @@
         <v>58.314938953868399</v>
       </c>
     </row>
-    <row r="168" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
         <v>6</v>
       </c>
@@ -5024,7 +5028,7 @@
         <v>58.046551808943001</v>
       </c>
     </row>
-    <row r="169" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
         <v>7</v>
       </c>
@@ -5050,7 +5054,7 @@
         <v>59.4720778187653</v>
       </c>
     </row>
-    <row r="170" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
         <v>20</v>
       </c>
@@ -5076,7 +5080,7 @@
         <v>61.278422356104898</v>
       </c>
     </row>
-    <row r="171" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
         <v>5</v>
       </c>
@@ -5102,7 +5106,7 @@
         <v>61.370063027329799</v>
       </c>
     </row>
-    <row r="172" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
         <v>6</v>
       </c>
@@ -5128,7 +5132,7 @@
         <v>62.103915439406897</v>
       </c>
     </row>
-    <row r="173" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
         <v>7</v>
       </c>
@@ -5154,7 +5158,7 @@
         <v>60.910570521699498</v>
       </c>
     </row>
-    <row r="174" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
         <v>20</v>
       </c>
@@ -5180,7 +5184,7 @@
         <v>59.730834236764601</v>
       </c>
     </row>
-    <row r="175" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
         <v>5</v>
       </c>
@@ -5206,7 +5210,7 @@
         <v>60.209678976188201</v>
       </c>
     </row>
-    <row r="176" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
         <v>6</v>
       </c>
@@ -5232,7 +5236,7 @@
         <v>59.896420192305399</v>
       </c>
     </row>
-    <row r="177" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
         <v>7</v>
       </c>
@@ -5258,7 +5262,7 @@
         <v>59.808368665338399</v>
       </c>
     </row>
-    <row r="178" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
         <v>20</v>
       </c>
@@ -5284,7 +5288,7 @@
         <v>78.285348619816702</v>
       </c>
     </row>
-    <row r="179" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
         <v>5</v>
       </c>
@@ -5310,7 +5314,7 @@
         <v>77.379577031305899</v>
       </c>
     </row>
-    <row r="180" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
         <v>6</v>
       </c>
@@ -5336,7 +5340,7 @@
         <v>78.918818993646298</v>
       </c>
     </row>
-    <row r="181" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
         <v>7</v>
       </c>
@@ -5362,7 +5366,7 @@
         <v>77.489846275260703</v>
       </c>
     </row>
-    <row r="182" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
         <v>20</v>
       </c>
@@ -5388,7 +5392,7 @@
         <v>71.731816440208405</v>
       </c>
     </row>
-    <row r="183" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
         <v>5</v>
       </c>
@@ -5414,7 +5418,7 @@
         <v>72.353090051195494</v>
       </c>
     </row>
-    <row r="184" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
         <v>6</v>
       </c>
@@ -5440,7 +5444,7 @@
         <v>69.772719346866495</v>
       </c>
     </row>
-    <row r="185" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
         <v>7</v>
       </c>
@@ -5466,7 +5470,7 @@
         <v>70.744810920936601</v>
       </c>
     </row>
-    <row r="186" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
         <v>20</v>
       </c>
@@ -5492,7 +5496,7 @@
         <v>72.3638012980756</v>
       </c>
     </row>
-    <row r="187" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
         <v>5</v>
       </c>
@@ -5518,7 +5522,7 @@
         <v>71.880607209367994</v>
       </c>
     </row>
-    <row r="188" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
         <v>6</v>
       </c>
@@ -5544,7 +5548,7 @@
         <v>70.042322618831804</v>
       </c>
     </row>
-    <row r="189" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
         <v>7</v>
       </c>
@@ -5570,7 +5574,7 @@
         <v>68.2094393134726</v>
       </c>
     </row>
-    <row r="190" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
         <v>20</v>
       </c>
@@ -5596,7 +5600,7 @@
         <v>68.319451458291596</v>
       </c>
     </row>
-    <row r="191" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
         <v>5</v>
       </c>
@@ -5622,7 +5626,7 @@
         <v>68.628440864837501</v>
       </c>
     </row>
-    <row r="192" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
         <v>6</v>
       </c>
@@ -5648,7 +5652,7 @@
         <v>69.382256928030898</v>
       </c>
     </row>
-    <row r="193" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
         <v>7</v>
       </c>
@@ -5674,7 +5678,7 @@
         <v>68.491844063995998</v>
       </c>
     </row>
-    <row r="194" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
         <v>20</v>
       </c>
@@ -5700,7 +5704,7 @@
         <v>61.779391084487898</v>
       </c>
     </row>
-    <row r="195" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
         <v>5</v>
       </c>
@@ -5726,7 +5730,7 @@
         <v>61.440889273312102</v>
       </c>
     </row>
-    <row r="196" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
         <v>6</v>
       </c>
@@ -5752,7 +5756,7 @@
         <v>62.854569048880897</v>
       </c>
     </row>
-    <row r="197" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
         <v>7</v>
       </c>
@@ -5778,7 +5782,7 @@
         <v>64.1248643568061</v>
       </c>
     </row>
-    <row r="198" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
         <v>20</v>
       </c>
@@ -5804,7 +5808,7 @@
         <v>62.207104416955602</v>
       </c>
     </row>
-    <row r="199" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
         <v>5</v>
       </c>
@@ -5830,7 +5834,7 @@
         <v>62.285196925718502</v>
       </c>
     </row>
-    <row r="200" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
         <v>6</v>
       </c>
@@ -5856,7 +5860,7 @@
         <v>62.7862902029037</v>
       </c>
     </row>
-    <row r="201" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
         <v>7</v>
       </c>
@@ -5882,7 +5886,7 @@
         <v>62.026260504145597</v>
       </c>
     </row>
-    <row r="202" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
         <v>16</v>
       </c>
@@ -5908,7 +5912,7 @@
         <v>63.41366</v>
       </c>
     </row>
-    <row r="203" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
         <v>17</v>
       </c>
@@ -5934,7 +5938,7 @@
         <v>63.219059999999999</v>
       </c>
     </row>
-    <row r="204" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
         <v>18</v>
       </c>
@@ -5960,7 +5964,7 @@
         <v>63.628909999999998</v>
       </c>
     </row>
-    <row r="205" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
         <v>19</v>
       </c>
@@ -5986,7 +5990,7 @@
         <v>63.658209999999997</v>
       </c>
     </row>
-    <row r="206" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
         <v>20</v>
       </c>
@@ -6012,7 +6016,7 @@
         <v>63.191679999999998</v>
       </c>
     </row>
-    <row r="207" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
         <v>5</v>
       </c>
@@ -6038,7 +6042,7 @@
         <v>63.760599999999997</v>
       </c>
     </row>
-    <row r="208" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
         <v>6</v>
       </c>
@@ -6064,7 +6068,7 @@
         <v>63.11985</v>
       </c>
     </row>
-    <row r="209" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
         <v>7</v>
       </c>
@@ -6090,7 +6094,7 @@
         <v>62.684420000000003</v>
       </c>
     </row>
-    <row r="210" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
         <v>16</v>
       </c>
@@ -6116,7 +6120,7 @@
         <v>61.413240000000002</v>
       </c>
     </row>
-    <row r="211" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
         <v>17</v>
       </c>
@@ -6142,7 +6146,7 @@
         <v>61.75638</v>
       </c>
     </row>
-    <row r="212" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A212" t="s">
         <v>18</v>
       </c>
@@ -6168,7 +6172,7 @@
         <v>62.041580000000003</v>
       </c>
     </row>
-    <row r="213" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A213" t="s">
         <v>19</v>
       </c>
@@ -6194,7 +6198,7 @@
         <v>62.126350000000002</v>
       </c>
     </row>
-    <row r="214" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A214" t="s">
         <v>20</v>
       </c>
@@ -6220,7 +6224,7 @@
         <v>62.242060000000002</v>
       </c>
     </row>
-    <row r="215" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A215" t="s">
         <v>5</v>
       </c>
@@ -6246,7 +6250,7 @@
         <v>62.637970000000003</v>
       </c>
     </row>
-    <row r="216" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A216" t="s">
         <v>6</v>
       </c>
@@ -6272,7 +6276,7 @@
         <v>62.740279999999998</v>
       </c>
     </row>
-    <row r="217" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A217" t="s">
         <v>7</v>
       </c>
@@ -6298,7 +6302,7 @@
         <v>62.29712</v>
       </c>
     </row>
-    <row r="218" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A218" t="s">
         <v>20</v>
       </c>
@@ -6324,7 +6328,7 @@
         <v>70.142922551566798</v>
       </c>
     </row>
-    <row r="219" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A219" t="s">
         <v>5</v>
       </c>
@@ -6350,7 +6354,7 @@
         <v>69.180238697027306</v>
       </c>
     </row>
-    <row r="220" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A220" t="s">
         <v>6</v>
       </c>
@@ -6376,7 +6380,7 @@
         <v>67.259491365589895</v>
       </c>
     </row>
-    <row r="221" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A221" t="s">
         <v>7</v>
       </c>
@@ -6402,7 +6406,7 @@
         <v>67.337959411402295</v>
       </c>
     </row>
-    <row r="222" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A222" t="s">
         <v>20</v>
       </c>
@@ -6428,7 +6432,7 @@
         <v>66.692829415438695</v>
       </c>
     </row>
-    <row r="223" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A223" t="s">
         <v>5</v>
       </c>
@@ -6454,7 +6458,7 @@
         <v>66.565785139467096</v>
       </c>
     </row>
-    <row r="224" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A224" t="s">
         <v>6</v>
       </c>
@@ -6480,7 +6484,7 @@
         <v>66.256056966455901</v>
       </c>
     </row>
-    <row r="225" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A225" t="s">
         <v>7</v>
       </c>
@@ -6506,7 +6510,7 @@
         <v>65.351931065586001</v>
       </c>
     </row>
-    <row r="226" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A226" t="s">
         <v>20</v>
       </c>
@@ -6532,7 +6536,7 @@
         <v>74.570998739740901</v>
       </c>
     </row>
-    <row r="227" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A227" t="s">
         <v>5</v>
       </c>
@@ -6558,7 +6562,7 @@
         <v>75.327997760794204</v>
       </c>
     </row>
-    <row r="228" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A228" t="s">
         <v>6</v>
       </c>
@@ -6584,7 +6588,7 @@
         <v>71.793324991166401</v>
       </c>
     </row>
-    <row r="229" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A229" t="s">
         <v>7</v>
       </c>
@@ -6610,7 +6614,7 @@
         <v>65.350056500026497</v>
       </c>
     </row>
-    <row r="230" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A230" t="s">
         <v>20</v>
       </c>
@@ -6636,7 +6640,7 @@
         <v>69.633352993536107</v>
       </c>
     </row>
-    <row r="231" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A231" t="s">
         <v>5</v>
       </c>
@@ -6662,7 +6666,7 @@
         <v>71.371454656814095</v>
       </c>
     </row>
-    <row r="232" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A232" t="s">
         <v>6</v>
       </c>
@@ -6688,7 +6692,7 @@
         <v>72.003737368182499</v>
       </c>
     </row>
-    <row r="233" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A233" t="s">
         <v>7</v>
       </c>
@@ -6714,7 +6718,7 @@
         <v>72.958322904994105</v>
       </c>
     </row>
-    <row r="234" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A234" t="s">
         <v>20</v>
       </c>
@@ -6740,7 +6744,7 @@
         <v>62.6892160096737</v>
       </c>
     </row>
-    <row r="235" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A235" t="s">
         <v>5</v>
       </c>
@@ -6766,7 +6770,7 @@
         <v>63.347891692794299</v>
       </c>
     </row>
-    <row r="236" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A236" t="s">
         <v>6</v>
       </c>
@@ -6792,7 +6796,7 @@
         <v>65.7249118994946</v>
       </c>
     </row>
-    <row r="237" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A237" t="s">
         <v>7</v>
       </c>
@@ -6818,7 +6822,7 @@
         <v>65.700598461900299</v>
       </c>
     </row>
-    <row r="238" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A238" t="s">
         <v>20</v>
       </c>
@@ -6844,7 +6848,7 @@
         <v>64.267068232735596</v>
       </c>
     </row>
-    <row r="239" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A239" t="s">
         <v>5</v>
       </c>
@@ -6870,7 +6874,7 @@
         <v>64.081157592196504</v>
       </c>
     </row>
-    <row r="240" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A240" t="s">
         <v>6</v>
       </c>
@@ -6896,7 +6900,7 @@
         <v>63.781491042256299</v>
       </c>
     </row>
-    <row r="241" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A241" t="s">
         <v>7</v>
       </c>
@@ -6922,7 +6926,7 @@
         <v>63.446336589898998</v>
       </c>
     </row>
-    <row r="242" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A242" t="s">
         <v>20</v>
       </c>
@@ -6948,7 +6952,7 @@
         <v>64.854229873022604</v>
       </c>
     </row>
-    <row r="243" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A243" t="s">
         <v>5</v>
       </c>
@@ -6974,7 +6978,7 @@
         <v>65.005358464987907</v>
       </c>
     </row>
-    <row r="244" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A244" t="s">
         <v>6</v>
       </c>
@@ -7000,7 +7004,7 @@
         <v>64.855571059759896</v>
       </c>
     </row>
-    <row r="245" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A245" t="s">
         <v>7</v>
       </c>
@@ -7026,7 +7030,7 @@
         <v>64.1930169126462</v>
       </c>
     </row>
-    <row r="246" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A246" t="s">
         <v>20</v>
       </c>
@@ -7052,7 +7056,7 @@
         <v>61.934782152564502</v>
       </c>
     </row>
-    <row r="247" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A247" t="s">
         <v>5</v>
       </c>
@@ -7078,7 +7082,7 @@
         <v>63.140813767795997</v>
       </c>
     </row>
-    <row r="248" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A248" t="s">
         <v>6</v>
       </c>
@@ -7104,7 +7108,7 @@
         <v>62.6139035404547</v>
       </c>
     </row>
-    <row r="249" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A249" t="s">
         <v>7</v>
       </c>
@@ -7130,7 +7134,7 @@
         <v>61.2225574653067</v>
       </c>
     </row>
-    <row r="250" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A250" t="s">
         <v>20</v>
       </c>
@@ -7156,7 +7160,7 @@
         <v>67.460160506828899</v>
       </c>
     </row>
-    <row r="251" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A251" t="s">
         <v>5</v>
       </c>
@@ -7182,7 +7186,7 @@
         <v>67.072905401698804</v>
       </c>
     </row>
-    <row r="252" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A252" t="s">
         <v>6</v>
       </c>
@@ -7208,7 +7212,7 @@
         <v>66.500591205195903</v>
       </c>
     </row>
-    <row r="253" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A253" t="s">
         <v>7</v>
       </c>
@@ -7234,7 +7238,7 @@
         <v>66.325991499510806</v>
       </c>
     </row>
-    <row r="254" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A254" t="s">
         <v>20</v>
       </c>
@@ -7260,7 +7264,7 @@
         <v>66.805053746284202</v>
       </c>
     </row>
-    <row r="255" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A255" t="s">
         <v>5</v>
       </c>
@@ -7286,7 +7290,7 @@
         <v>66.782371244404303</v>
       </c>
     </row>
-    <row r="256" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A256" t="s">
         <v>6</v>
       </c>
@@ -7312,7 +7316,7 @@
         <v>66.809187073804296</v>
       </c>
     </row>
-    <row r="257" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A257" t="s">
         <v>7</v>
       </c>
@@ -7338,7 +7342,7 @@
         <v>65.430475806172296</v>
       </c>
     </row>
-    <row r="258" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A258" t="s">
         <v>20</v>
       </c>
@@ -7364,7 +7368,7 @@
         <v>60.480439361315902</v>
       </c>
     </row>
-    <row r="259" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A259" t="s">
         <v>5</v>
       </c>
@@ -7390,7 +7394,7 @@
         <v>59.837720240978001</v>
       </c>
     </row>
-    <row r="260" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A260" t="s">
         <v>6</v>
       </c>
@@ -7416,7 +7420,7 @@
         <v>61.414121108859199</v>
       </c>
     </row>
-    <row r="261" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A261" t="s">
         <v>7</v>
       </c>
@@ -7442,7 +7446,7 @@
         <v>62.387226837184102</v>
       </c>
     </row>
-    <row r="262" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A262" t="s">
         <v>20</v>
       </c>
@@ -7468,7 +7472,7 @@
         <v>58.688774272539902</v>
       </c>
     </row>
-    <row r="263" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A263" t="s">
         <v>5</v>
       </c>
@@ -7494,7 +7498,7 @@
         <v>57.742205193421803</v>
       </c>
     </row>
-    <row r="264" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A264" t="s">
         <v>6</v>
       </c>
@@ -7520,7 +7524,7 @@
         <v>60.026712817030301</v>
       </c>
     </row>
-    <row r="265" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A265" t="s">
         <v>7</v>
       </c>
@@ -7546,7 +7550,7 @@
         <v>60.085854040065598</v>
       </c>
     </row>
-    <row r="266" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A266" t="s">
         <v>20</v>
       </c>
@@ -7572,7 +7576,7 @@
         <v>60.905370410499501</v>
       </c>
     </row>
-    <row r="267" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A267" t="s">
         <v>5</v>
       </c>
@@ -7598,7 +7602,7 @@
         <v>63.385491850652301</v>
       </c>
     </row>
-    <row r="268" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A268" t="s">
         <v>6</v>
       </c>
@@ -7624,7 +7628,7 @@
         <v>64.391575345260094</v>
       </c>
     </row>
-    <row r="269" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A269" t="s">
         <v>7</v>
       </c>
@@ -7650,7 +7654,7 @@
         <v>64.062574353995601</v>
       </c>
     </row>
-    <row r="270" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A270" t="s">
         <v>20</v>
       </c>
@@ -7676,7 +7680,7 @@
         <v>64.383020917420197</v>
       </c>
     </row>
-    <row r="271" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A271" t="s">
         <v>5</v>
       </c>
@@ -7702,7 +7706,7 @@
         <v>64.286458254260396</v>
       </c>
     </row>
-    <row r="272" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A272" t="s">
         <v>6</v>
       </c>
@@ -7728,7 +7732,7 @@
         <v>64.123652744958306</v>
       </c>
     </row>
-    <row r="273" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A273" t="s">
         <v>7</v>
       </c>
@@ -7754,8 +7758,1724 @@
         <v>65.028851547390403</v>
       </c>
     </row>
+    <row r="274" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A274" t="s">
+        <v>85</v>
+      </c>
+      <c r="B274" t="s">
+        <v>21</v>
+      </c>
+      <c r="C274" t="s">
+        <v>22</v>
+      </c>
+      <c r="D274" t="s">
+        <v>0</v>
+      </c>
+      <c r="E274" t="s">
+        <v>1</v>
+      </c>
+      <c r="F274">
+        <v>62.78</v>
+      </c>
+      <c r="G274">
+        <v>60.38</v>
+      </c>
+      <c r="H274">
+        <v>65.19</v>
+      </c>
+    </row>
+    <row r="275" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A275" t="s">
+        <v>85</v>
+      </c>
+      <c r="B275" t="s">
+        <v>21</v>
+      </c>
+      <c r="C275" t="s">
+        <v>22</v>
+      </c>
+      <c r="D275" t="s">
+        <v>2</v>
+      </c>
+      <c r="E275" t="s">
+        <v>1</v>
+      </c>
+      <c r="F275">
+        <v>62.41</v>
+      </c>
+      <c r="G275">
+        <v>59.35</v>
+      </c>
+      <c r="H275">
+        <v>65.47</v>
+      </c>
+    </row>
+    <row r="276" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A276" t="s">
+        <v>85</v>
+      </c>
+      <c r="B276" t="s">
+        <v>23</v>
+      </c>
+      <c r="C276" t="s">
+        <v>24</v>
+      </c>
+      <c r="D276" t="s">
+        <v>0</v>
+      </c>
+      <c r="E276" t="s">
+        <v>1</v>
+      </c>
+      <c r="F276">
+        <v>62.39</v>
+      </c>
+      <c r="G276">
+        <v>60.57</v>
+      </c>
+      <c r="H276">
+        <v>64.22</v>
+      </c>
+    </row>
+    <row r="277" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A277" t="s">
+        <v>85</v>
+      </c>
+      <c r="B277" t="s">
+        <v>23</v>
+      </c>
+      <c r="C277" t="s">
+        <v>24</v>
+      </c>
+      <c r="D277" t="s">
+        <v>2</v>
+      </c>
+      <c r="E277" t="s">
+        <v>1</v>
+      </c>
+      <c r="F277">
+        <v>62.53</v>
+      </c>
+      <c r="G277">
+        <v>60.32</v>
+      </c>
+      <c r="H277">
+        <v>64.739999999999995</v>
+      </c>
+    </row>
+    <row r="278" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A278" t="s">
+        <v>85</v>
+      </c>
+      <c r="B278" t="s">
+        <v>25</v>
+      </c>
+      <c r="C278" t="s">
+        <v>26</v>
+      </c>
+      <c r="D278" t="s">
+        <v>0</v>
+      </c>
+      <c r="E278" t="s">
+        <v>1</v>
+      </c>
+      <c r="F278">
+        <v>59.33</v>
+      </c>
+      <c r="G278">
+        <v>57.47</v>
+      </c>
+      <c r="H278">
+        <v>61.19</v>
+      </c>
+    </row>
+    <row r="279" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A279" t="s">
+        <v>85</v>
+      </c>
+      <c r="B279" t="s">
+        <v>25</v>
+      </c>
+      <c r="C279" t="s">
+        <v>26</v>
+      </c>
+      <c r="D279" t="s">
+        <v>2</v>
+      </c>
+      <c r="E279" t="s">
+        <v>1</v>
+      </c>
+      <c r="F279">
+        <v>58.24</v>
+      </c>
+      <c r="G279">
+        <v>56.07</v>
+      </c>
+      <c r="H279">
+        <v>60.41</v>
+      </c>
+    </row>
+    <row r="280" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A280" t="s">
+        <v>85</v>
+      </c>
+      <c r="B280" t="s">
+        <v>27</v>
+      </c>
+      <c r="C280" t="s">
+        <v>28</v>
+      </c>
+      <c r="D280" t="s">
+        <v>0</v>
+      </c>
+      <c r="E280" t="s">
+        <v>1</v>
+      </c>
+      <c r="F280">
+        <v>65.2</v>
+      </c>
+      <c r="G280">
+        <v>63.25</v>
+      </c>
+      <c r="H280">
+        <v>67.150000000000006</v>
+      </c>
+    </row>
+    <row r="281" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A281" t="s">
+        <v>85</v>
+      </c>
+      <c r="B281" t="s">
+        <v>27</v>
+      </c>
+      <c r="C281" t="s">
+        <v>28</v>
+      </c>
+      <c r="D281" t="s">
+        <v>2</v>
+      </c>
+      <c r="E281" t="s">
+        <v>1</v>
+      </c>
+      <c r="F281">
+        <v>64.61</v>
+      </c>
+      <c r="G281">
+        <v>62.47</v>
+      </c>
+      <c r="H281">
+        <v>66.75</v>
+      </c>
+    </row>
+    <row r="282" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A282" t="s">
+        <v>85</v>
+      </c>
+      <c r="B282" t="s">
+        <v>29</v>
+      </c>
+      <c r="C282" t="s">
+        <v>30</v>
+      </c>
+      <c r="D282" t="s">
+        <v>0</v>
+      </c>
+      <c r="E282" t="s">
+        <v>1</v>
+      </c>
+      <c r="F282">
+        <v>68.28</v>
+      </c>
+      <c r="G282">
+        <v>66.44</v>
+      </c>
+      <c r="H282">
+        <v>70.13</v>
+      </c>
+    </row>
+    <row r="283" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A283" t="s">
+        <v>85</v>
+      </c>
+      <c r="B283" t="s">
+        <v>29</v>
+      </c>
+      <c r="C283" t="s">
+        <v>30</v>
+      </c>
+      <c r="D283" t="s">
+        <v>2</v>
+      </c>
+      <c r="E283" t="s">
+        <v>1</v>
+      </c>
+      <c r="F283">
+        <v>67.19</v>
+      </c>
+      <c r="G283">
+        <v>65.040000000000006</v>
+      </c>
+      <c r="H283">
+        <v>69.33</v>
+      </c>
+    </row>
+    <row r="284" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A284" t="s">
+        <v>85</v>
+      </c>
+      <c r="B284" t="s">
+        <v>31</v>
+      </c>
+      <c r="C284" t="s">
+        <v>32</v>
+      </c>
+      <c r="D284" t="s">
+        <v>0</v>
+      </c>
+      <c r="E284" t="s">
+        <v>1</v>
+      </c>
+      <c r="F284">
+        <v>66.989999999999995</v>
+      </c>
+      <c r="G284">
+        <v>64.069999999999993</v>
+      </c>
+      <c r="H284">
+        <v>69.92</v>
+      </c>
+    </row>
+    <row r="285" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A285" t="s">
+        <v>85</v>
+      </c>
+      <c r="B285" t="s">
+        <v>31</v>
+      </c>
+      <c r="C285" t="s">
+        <v>32</v>
+      </c>
+      <c r="D285" t="s">
+        <v>2</v>
+      </c>
+      <c r="E285" t="s">
+        <v>1</v>
+      </c>
+      <c r="F285">
+        <v>69.58</v>
+      </c>
+      <c r="G285">
+        <v>66.760000000000005</v>
+      </c>
+      <c r="H285">
+        <v>72.400000000000006</v>
+      </c>
+    </row>
+    <row r="286" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A286" t="s">
+        <v>85</v>
+      </c>
+      <c r="B286" t="s">
+        <v>33</v>
+      </c>
+      <c r="C286" t="s">
+        <v>34</v>
+      </c>
+      <c r="D286" t="s">
+        <v>0</v>
+      </c>
+      <c r="E286" t="s">
+        <v>1</v>
+      </c>
+      <c r="F286">
+        <v>62.39</v>
+      </c>
+      <c r="G286">
+        <v>60.66</v>
+      </c>
+      <c r="H286">
+        <v>64.12</v>
+      </c>
+    </row>
+    <row r="287" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A287" t="s">
+        <v>85</v>
+      </c>
+      <c r="B287" t="s">
+        <v>33</v>
+      </c>
+      <c r="C287" t="s">
+        <v>34</v>
+      </c>
+      <c r="D287" t="s">
+        <v>2</v>
+      </c>
+      <c r="E287" t="s">
+        <v>1</v>
+      </c>
+      <c r="F287">
+        <v>59.71</v>
+      </c>
+      <c r="G287">
+        <v>57.8</v>
+      </c>
+      <c r="H287">
+        <v>61.63</v>
+      </c>
+    </row>
+    <row r="288" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A288" t="s">
+        <v>85</v>
+      </c>
+      <c r="B288" t="s">
+        <v>35</v>
+      </c>
+      <c r="C288" t="s">
+        <v>36</v>
+      </c>
+      <c r="D288" t="s">
+        <v>0</v>
+      </c>
+      <c r="E288" t="s">
+        <v>1</v>
+      </c>
+      <c r="F288">
+        <v>63.95</v>
+      </c>
+      <c r="G288">
+        <v>61.95</v>
+      </c>
+      <c r="H288">
+        <v>65.94</v>
+      </c>
+    </row>
+    <row r="289" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A289" t="s">
+        <v>85</v>
+      </c>
+      <c r="B289" t="s">
+        <v>35</v>
+      </c>
+      <c r="C289" t="s">
+        <v>36</v>
+      </c>
+      <c r="D289" t="s">
+        <v>2</v>
+      </c>
+      <c r="E289" t="s">
+        <v>1</v>
+      </c>
+      <c r="F289">
+        <v>64.36</v>
+      </c>
+      <c r="G289">
+        <v>61.6</v>
+      </c>
+      <c r="H289">
+        <v>67.12</v>
+      </c>
+    </row>
+    <row r="290" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A290" t="s">
+        <v>85</v>
+      </c>
+      <c r="B290" t="s">
+        <v>37</v>
+      </c>
+      <c r="C290" t="s">
+        <v>38</v>
+      </c>
+      <c r="D290" t="s">
+        <v>0</v>
+      </c>
+      <c r="E290" t="s">
+        <v>1</v>
+      </c>
+      <c r="F290">
+        <v>58.35</v>
+      </c>
+      <c r="G290">
+        <v>56.38</v>
+      </c>
+      <c r="H290">
+        <v>60.32</v>
+      </c>
+    </row>
+    <row r="291" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A291" t="s">
+        <v>85</v>
+      </c>
+      <c r="B291" t="s">
+        <v>37</v>
+      </c>
+      <c r="C291" t="s">
+        <v>38</v>
+      </c>
+      <c r="D291" t="s">
+        <v>2</v>
+      </c>
+      <c r="E291" t="s">
+        <v>1</v>
+      </c>
+      <c r="F291">
+        <v>59.65</v>
+      </c>
+      <c r="G291">
+        <v>57.62</v>
+      </c>
+      <c r="H291">
+        <v>61.69</v>
+      </c>
+    </row>
+    <row r="292" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A292" t="s">
+        <v>85</v>
+      </c>
+      <c r="B292" t="s">
+        <v>39</v>
+      </c>
+      <c r="C292" t="s">
+        <v>40</v>
+      </c>
+      <c r="D292" t="s">
+        <v>0</v>
+      </c>
+      <c r="E292" t="s">
+        <v>1</v>
+      </c>
+      <c r="F292">
+        <v>63.36</v>
+      </c>
+      <c r="G292">
+        <v>61.13</v>
+      </c>
+      <c r="H292">
+        <v>65.59</v>
+      </c>
+    </row>
+    <row r="293" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A293" t="s">
+        <v>85</v>
+      </c>
+      <c r="B293" t="s">
+        <v>39</v>
+      </c>
+      <c r="C293" t="s">
+        <v>40</v>
+      </c>
+      <c r="D293" t="s">
+        <v>2</v>
+      </c>
+      <c r="E293" t="s">
+        <v>1</v>
+      </c>
+      <c r="F293">
+        <v>63.97</v>
+      </c>
+      <c r="G293">
+        <v>61.64</v>
+      </c>
+      <c r="H293">
+        <v>66.290000000000006</v>
+      </c>
+    </row>
+    <row r="294" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A294" t="s">
+        <v>85</v>
+      </c>
+      <c r="B294" t="s">
+        <v>41</v>
+      </c>
+      <c r="C294" t="s">
+        <v>42</v>
+      </c>
+      <c r="D294" t="s">
+        <v>0</v>
+      </c>
+      <c r="E294" t="s">
+        <v>1</v>
+      </c>
+      <c r="F294">
+        <v>61.48</v>
+      </c>
+      <c r="G294">
+        <v>59.53</v>
+      </c>
+      <c r="H294">
+        <v>63.43</v>
+      </c>
+    </row>
+    <row r="295" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A295" t="s">
+        <v>85</v>
+      </c>
+      <c r="B295" t="s">
+        <v>41</v>
+      </c>
+      <c r="C295" t="s">
+        <v>42</v>
+      </c>
+      <c r="D295" t="s">
+        <v>2</v>
+      </c>
+      <c r="E295" t="s">
+        <v>1</v>
+      </c>
+      <c r="F295">
+        <v>61.38</v>
+      </c>
+      <c r="G295">
+        <v>58.98</v>
+      </c>
+      <c r="H295">
+        <v>63.78</v>
+      </c>
+    </row>
+    <row r="296" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A296" t="s">
+        <v>85</v>
+      </c>
+      <c r="B296" t="s">
+        <v>43</v>
+      </c>
+      <c r="C296" t="s">
+        <v>44</v>
+      </c>
+      <c r="D296" t="s">
+        <v>0</v>
+      </c>
+      <c r="E296" t="s">
+        <v>1</v>
+      </c>
+      <c r="F296">
+        <v>58.52</v>
+      </c>
+      <c r="G296">
+        <v>56.58</v>
+      </c>
+      <c r="H296">
+        <v>60.46</v>
+      </c>
+    </row>
+    <row r="297" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A297" t="s">
+        <v>85</v>
+      </c>
+      <c r="B297" t="s">
+        <v>43</v>
+      </c>
+      <c r="C297" t="s">
+        <v>44</v>
+      </c>
+      <c r="D297" t="s">
+        <v>2</v>
+      </c>
+      <c r="E297" t="s">
+        <v>1</v>
+      </c>
+      <c r="F297">
+        <v>56.34</v>
+      </c>
+      <c r="G297">
+        <v>54.23</v>
+      </c>
+      <c r="H297">
+        <v>58.44</v>
+      </c>
+    </row>
+    <row r="298" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A298" t="s">
+        <v>85</v>
+      </c>
+      <c r="B298" t="s">
+        <v>45</v>
+      </c>
+      <c r="C298" t="s">
+        <v>46</v>
+      </c>
+      <c r="D298" t="s">
+        <v>0</v>
+      </c>
+      <c r="E298" t="s">
+        <v>1</v>
+      </c>
+      <c r="F298">
+        <v>69.33</v>
+      </c>
+      <c r="G298">
+        <v>65.599999999999994</v>
+      </c>
+      <c r="H298">
+        <v>73.069999999999993</v>
+      </c>
+    </row>
+    <row r="299" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A299" t="s">
+        <v>85</v>
+      </c>
+      <c r="B299" t="s">
+        <v>45</v>
+      </c>
+      <c r="C299" t="s">
+        <v>46</v>
+      </c>
+      <c r="D299" t="s">
+        <v>2</v>
+      </c>
+      <c r="E299" t="s">
+        <v>1</v>
+      </c>
+      <c r="F299">
+        <v>75.05</v>
+      </c>
+      <c r="G299">
+        <v>71.37</v>
+      </c>
+      <c r="H299">
+        <v>78.73</v>
+      </c>
+    </row>
+    <row r="300" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A300" t="s">
+        <v>85</v>
+      </c>
+      <c r="B300" t="s">
+        <v>47</v>
+      </c>
+      <c r="C300" t="s">
+        <v>48</v>
+      </c>
+      <c r="D300" t="s">
+        <v>0</v>
+      </c>
+      <c r="E300" t="s">
+        <v>1</v>
+      </c>
+      <c r="F300">
+        <v>63.31</v>
+      </c>
+      <c r="G300">
+        <v>61.41</v>
+      </c>
+      <c r="H300">
+        <v>65.209999999999994</v>
+      </c>
+    </row>
+    <row r="301" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A301" t="s">
+        <v>85</v>
+      </c>
+      <c r="B301" t="s">
+        <v>47</v>
+      </c>
+      <c r="C301" t="s">
+        <v>48</v>
+      </c>
+      <c r="D301" t="s">
+        <v>2</v>
+      </c>
+      <c r="E301" t="s">
+        <v>1</v>
+      </c>
+      <c r="F301">
+        <v>63.81</v>
+      </c>
+      <c r="G301">
+        <v>61.68</v>
+      </c>
+      <c r="H301">
+        <v>65.95</v>
+      </c>
+    </row>
+    <row r="302" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A302" t="s">
+        <v>85</v>
+      </c>
+      <c r="B302" t="s">
+        <v>49</v>
+      </c>
+      <c r="C302" t="s">
+        <v>50</v>
+      </c>
+      <c r="D302" t="s">
+        <v>0</v>
+      </c>
+      <c r="E302" t="s">
+        <v>1</v>
+      </c>
+      <c r="F302">
+        <v>68.95</v>
+      </c>
+      <c r="G302">
+        <v>62.71</v>
+      </c>
+      <c r="H302">
+        <v>75.2</v>
+      </c>
+    </row>
+    <row r="303" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A303" t="s">
+        <v>85</v>
+      </c>
+      <c r="B303" t="s">
+        <v>49</v>
+      </c>
+      <c r="C303" t="s">
+        <v>50</v>
+      </c>
+      <c r="D303" t="s">
+        <v>2</v>
+      </c>
+      <c r="E303" t="s">
+        <v>1</v>
+      </c>
+      <c r="F303">
+        <v>61.87</v>
+      </c>
+      <c r="G303">
+        <v>55.71</v>
+      </c>
+      <c r="H303">
+        <v>68.03</v>
+      </c>
+    </row>
+    <row r="304" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A304" t="s">
+        <v>85</v>
+      </c>
+      <c r="B304" t="s">
+        <v>51</v>
+      </c>
+      <c r="C304" t="s">
+        <v>52</v>
+      </c>
+      <c r="D304" t="s">
+        <v>0</v>
+      </c>
+      <c r="E304" t="s">
+        <v>1</v>
+      </c>
+      <c r="F304">
+        <v>59.96</v>
+      </c>
+      <c r="G304">
+        <v>58</v>
+      </c>
+      <c r="H304">
+        <v>61.93</v>
+      </c>
+    </row>
+    <row r="305" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A305" t="s">
+        <v>85</v>
+      </c>
+      <c r="B305" t="s">
+        <v>51</v>
+      </c>
+      <c r="C305" t="s">
+        <v>52</v>
+      </c>
+      <c r="D305" t="s">
+        <v>2</v>
+      </c>
+      <c r="E305" t="s">
+        <v>1</v>
+      </c>
+      <c r="F305">
+        <v>63.28</v>
+      </c>
+      <c r="G305">
+        <v>61.05</v>
+      </c>
+      <c r="H305">
+        <v>65.5</v>
+      </c>
+    </row>
+    <row r="306" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A306" t="s">
+        <v>85</v>
+      </c>
+      <c r="B306" t="s">
+        <v>53</v>
+      </c>
+      <c r="C306" t="s">
+        <v>54</v>
+      </c>
+      <c r="D306" t="s">
+        <v>0</v>
+      </c>
+      <c r="E306" t="s">
+        <v>1</v>
+      </c>
+      <c r="F306">
+        <v>57.91</v>
+      </c>
+      <c r="G306">
+        <v>55.95</v>
+      </c>
+      <c r="H306">
+        <v>59.86</v>
+      </c>
+    </row>
+    <row r="307" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A307" t="s">
+        <v>85</v>
+      </c>
+      <c r="B307" t="s">
+        <v>53</v>
+      </c>
+      <c r="C307" t="s">
+        <v>54</v>
+      </c>
+      <c r="D307" t="s">
+        <v>2</v>
+      </c>
+      <c r="E307" t="s">
+        <v>1</v>
+      </c>
+      <c r="F307">
+        <v>62.98</v>
+      </c>
+      <c r="G307">
+        <v>61.02</v>
+      </c>
+      <c r="H307">
+        <v>64.94</v>
+      </c>
+    </row>
+    <row r="308" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A308" t="s">
+        <v>85</v>
+      </c>
+      <c r="B308" t="s">
+        <v>55</v>
+      </c>
+      <c r="C308" t="s">
+        <v>56</v>
+      </c>
+      <c r="D308" t="s">
+        <v>0</v>
+      </c>
+      <c r="E308" t="s">
+        <v>1</v>
+      </c>
+      <c r="F308">
+        <v>61.79</v>
+      </c>
+      <c r="G308">
+        <v>59.63</v>
+      </c>
+      <c r="H308">
+        <v>63.94</v>
+      </c>
+    </row>
+    <row r="309" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A309" t="s">
+        <v>85</v>
+      </c>
+      <c r="B309" t="s">
+        <v>55</v>
+      </c>
+      <c r="C309" t="s">
+        <v>56</v>
+      </c>
+      <c r="D309" t="s">
+        <v>2</v>
+      </c>
+      <c r="E309" t="s">
+        <v>1</v>
+      </c>
+      <c r="F309">
+        <v>64.900000000000006</v>
+      </c>
+      <c r="G309">
+        <v>62.97</v>
+      </c>
+      <c r="H309">
+        <v>66.819999999999993</v>
+      </c>
+    </row>
+    <row r="310" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A310" t="s">
+        <v>85</v>
+      </c>
+      <c r="B310" t="s">
+        <v>57</v>
+      </c>
+      <c r="C310" t="s">
+        <v>58</v>
+      </c>
+      <c r="D310" t="s">
+        <v>0</v>
+      </c>
+      <c r="E310" t="s">
+        <v>1</v>
+      </c>
+      <c r="F310">
+        <v>60.59</v>
+      </c>
+      <c r="G310">
+        <v>58.46</v>
+      </c>
+      <c r="H310">
+        <v>62.71</v>
+      </c>
+    </row>
+    <row r="311" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A311" t="s">
+        <v>85</v>
+      </c>
+      <c r="B311" t="s">
+        <v>57</v>
+      </c>
+      <c r="C311" t="s">
+        <v>58</v>
+      </c>
+      <c r="D311" t="s">
+        <v>2</v>
+      </c>
+      <c r="E311" t="s">
+        <v>1</v>
+      </c>
+      <c r="F311">
+        <v>62.52</v>
+      </c>
+      <c r="G311">
+        <v>60.05</v>
+      </c>
+      <c r="H311">
+        <v>64.98</v>
+      </c>
+    </row>
+    <row r="312" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A312" t="s">
+        <v>85</v>
+      </c>
+      <c r="B312" t="s">
+        <v>59</v>
+      </c>
+      <c r="C312" t="s">
+        <v>60</v>
+      </c>
+      <c r="D312" t="s">
+        <v>0</v>
+      </c>
+      <c r="E312" t="s">
+        <v>1</v>
+      </c>
+      <c r="F312">
+        <v>67.91</v>
+      </c>
+      <c r="G312">
+        <v>66.209999999999994</v>
+      </c>
+      <c r="H312">
+        <v>69.61</v>
+      </c>
+    </row>
+    <row r="313" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A313" t="s">
+        <v>85</v>
+      </c>
+      <c r="B313" t="s">
+        <v>59</v>
+      </c>
+      <c r="C313" t="s">
+        <v>60</v>
+      </c>
+      <c r="D313" t="s">
+        <v>2</v>
+      </c>
+      <c r="E313" t="s">
+        <v>1</v>
+      </c>
+      <c r="F313">
+        <v>65.959999999999994</v>
+      </c>
+      <c r="G313">
+        <v>63.73</v>
+      </c>
+      <c r="H313">
+        <v>68.180000000000007</v>
+      </c>
+    </row>
+    <row r="314" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A314" t="s">
+        <v>85</v>
+      </c>
+      <c r="B314" t="s">
+        <v>61</v>
+      </c>
+      <c r="C314" t="s">
+        <v>62</v>
+      </c>
+      <c r="D314" t="s">
+        <v>0</v>
+      </c>
+      <c r="E314" t="s">
+        <v>1</v>
+      </c>
+      <c r="F314">
+        <v>64.7</v>
+      </c>
+      <c r="G314">
+        <v>63.02</v>
+      </c>
+      <c r="H314">
+        <v>66.37</v>
+      </c>
+    </row>
+    <row r="315" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A315" t="s">
+        <v>85</v>
+      </c>
+      <c r="B315" t="s">
+        <v>61</v>
+      </c>
+      <c r="C315" t="s">
+        <v>62</v>
+      </c>
+      <c r="D315" t="s">
+        <v>2</v>
+      </c>
+      <c r="E315" t="s">
+        <v>1</v>
+      </c>
+      <c r="F315">
+        <v>63.43</v>
+      </c>
+      <c r="G315">
+        <v>61.42</v>
+      </c>
+      <c r="H315">
+        <v>65.45</v>
+      </c>
+    </row>
+    <row r="316" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A316" t="s">
+        <v>85</v>
+      </c>
+      <c r="B316" t="s">
+        <v>63</v>
+      </c>
+      <c r="C316" t="s">
+        <v>64</v>
+      </c>
+      <c r="D316" t="s">
+        <v>0</v>
+      </c>
+      <c r="E316" t="s">
+        <v>1</v>
+      </c>
+      <c r="F316">
+        <v>66.290000000000006</v>
+      </c>
+      <c r="G316">
+        <v>64.42</v>
+      </c>
+      <c r="H316">
+        <v>68.16</v>
+      </c>
+    </row>
+    <row r="317" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A317" t="s">
+        <v>85</v>
+      </c>
+      <c r="B317" t="s">
+        <v>63</v>
+      </c>
+      <c r="C317" t="s">
+        <v>64</v>
+      </c>
+      <c r="D317" t="s">
+        <v>2</v>
+      </c>
+      <c r="E317" t="s">
+        <v>1</v>
+      </c>
+      <c r="F317">
+        <v>64.989999999999995</v>
+      </c>
+      <c r="G317">
+        <v>62.94</v>
+      </c>
+      <c r="H317">
+        <v>67.05</v>
+      </c>
+    </row>
+    <row r="318" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A318" t="s">
+        <v>85</v>
+      </c>
+      <c r="B318" t="s">
+        <v>65</v>
+      </c>
+      <c r="C318" t="s">
+        <v>66</v>
+      </c>
+      <c r="D318" t="s">
+        <v>0</v>
+      </c>
+      <c r="E318" t="s">
+        <v>1</v>
+      </c>
+      <c r="F318">
+        <v>60.74</v>
+      </c>
+      <c r="G318">
+        <v>58.77</v>
+      </c>
+      <c r="H318">
+        <v>62.71</v>
+      </c>
+    </row>
+    <row r="319" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A319" t="s">
+        <v>85</v>
+      </c>
+      <c r="B319" t="s">
+        <v>65</v>
+      </c>
+      <c r="C319" t="s">
+        <v>66</v>
+      </c>
+      <c r="D319" t="s">
+        <v>2</v>
+      </c>
+      <c r="E319" t="s">
+        <v>1</v>
+      </c>
+      <c r="F319">
+        <v>62.26</v>
+      </c>
+      <c r="G319">
+        <v>60.15</v>
+      </c>
+      <c r="H319">
+        <v>64.36</v>
+      </c>
+    </row>
+    <row r="320" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A320" t="s">
+        <v>85</v>
+      </c>
+      <c r="B320" t="s">
+        <v>67</v>
+      </c>
+      <c r="C320" t="s">
+        <v>68</v>
+      </c>
+      <c r="D320" t="s">
+        <v>0</v>
+      </c>
+      <c r="E320" t="s">
+        <v>1</v>
+      </c>
+      <c r="F320">
+        <v>59.13</v>
+      </c>
+      <c r="G320">
+        <v>57.47</v>
+      </c>
+      <c r="H320">
+        <v>60.79</v>
+      </c>
+    </row>
+    <row r="321" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A321" t="s">
+        <v>85</v>
+      </c>
+      <c r="B321" t="s">
+        <v>67</v>
+      </c>
+      <c r="C321" t="s">
+        <v>68</v>
+      </c>
+      <c r="D321" t="s">
+        <v>2</v>
+      </c>
+      <c r="E321" t="s">
+        <v>1</v>
+      </c>
+      <c r="F321">
+        <v>60.55</v>
+      </c>
+      <c r="G321">
+        <v>58.81</v>
+      </c>
+      <c r="H321">
+        <v>62.29</v>
+      </c>
+    </row>
+    <row r="322" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A322" t="s">
+        <v>85</v>
+      </c>
+      <c r="B322" t="s">
+        <v>69</v>
+      </c>
+      <c r="C322" t="s">
+        <v>70</v>
+      </c>
+      <c r="D322" t="s">
+        <v>0</v>
+      </c>
+      <c r="E322" t="s">
+        <v>1</v>
+      </c>
+      <c r="F322">
+        <v>61.33</v>
+      </c>
+      <c r="G322">
+        <v>59.31</v>
+      </c>
+      <c r="H322">
+        <v>63.35</v>
+      </c>
+    </row>
+    <row r="323" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A323" t="s">
+        <v>85</v>
+      </c>
+      <c r="B323" t="s">
+        <v>69</v>
+      </c>
+      <c r="C323" t="s">
+        <v>70</v>
+      </c>
+      <c r="D323" t="s">
+        <v>2</v>
+      </c>
+      <c r="E323" t="s">
+        <v>1</v>
+      </c>
+      <c r="F323">
+        <v>59.07</v>
+      </c>
+      <c r="G323">
+        <v>56.96</v>
+      </c>
+      <c r="H323">
+        <v>61.18</v>
+      </c>
+    </row>
+    <row r="324" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A324" t="s">
+        <v>85</v>
+      </c>
+      <c r="B324" t="s">
+        <v>71</v>
+      </c>
+      <c r="C324" t="s">
+        <v>72</v>
+      </c>
+      <c r="D324" t="s">
+        <v>0</v>
+      </c>
+      <c r="E324" t="s">
+        <v>1</v>
+      </c>
+      <c r="F324">
+        <v>60.98</v>
+      </c>
+      <c r="G324">
+        <v>58.85</v>
+      </c>
+      <c r="H324">
+        <v>63.11</v>
+      </c>
+    </row>
+    <row r="325" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A325" t="s">
+        <v>85</v>
+      </c>
+      <c r="B325" t="s">
+        <v>71</v>
+      </c>
+      <c r="C325" t="s">
+        <v>72</v>
+      </c>
+      <c r="D325" t="s">
+        <v>2</v>
+      </c>
+      <c r="E325" t="s">
+        <v>1</v>
+      </c>
+      <c r="F325">
+        <v>63.09</v>
+      </c>
+      <c r="G325">
+        <v>60.98</v>
+      </c>
+      <c r="H325">
+        <v>65.19</v>
+      </c>
+    </row>
+    <row r="326" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A326" t="s">
+        <v>85</v>
+      </c>
+      <c r="B326" t="s">
+        <v>73</v>
+      </c>
+      <c r="C326" t="s">
+        <v>74</v>
+      </c>
+      <c r="D326" t="s">
+        <v>0</v>
+      </c>
+      <c r="E326" t="s">
+        <v>1</v>
+      </c>
+      <c r="F326">
+        <v>56.84</v>
+      </c>
+      <c r="G326">
+        <v>54.95</v>
+      </c>
+      <c r="H326">
+        <v>58.74</v>
+      </c>
+    </row>
+    <row r="327" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A327" t="s">
+        <v>85</v>
+      </c>
+      <c r="B327" t="s">
+        <v>73</v>
+      </c>
+      <c r="C327" t="s">
+        <v>74</v>
+      </c>
+      <c r="D327" t="s">
+        <v>2</v>
+      </c>
+      <c r="E327" t="s">
+        <v>1</v>
+      </c>
+      <c r="F327">
+        <v>57.88</v>
+      </c>
+      <c r="G327">
+        <v>55.74</v>
+      </c>
+      <c r="H327">
+        <v>60.02</v>
+      </c>
+    </row>
+    <row r="328" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A328" t="s">
+        <v>85</v>
+      </c>
+      <c r="B328" t="s">
+        <v>77</v>
+      </c>
+      <c r="C328" t="s">
+        <v>78</v>
+      </c>
+      <c r="D328" t="s">
+        <v>0</v>
+      </c>
+      <c r="E328" t="s">
+        <v>1</v>
+      </c>
+      <c r="F328">
+        <v>69.81</v>
+      </c>
+      <c r="G328">
+        <v>68.38</v>
+      </c>
+      <c r="H328">
+        <v>71.25</v>
+      </c>
+    </row>
+    <row r="329" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A329" t="s">
+        <v>85</v>
+      </c>
+      <c r="B329" t="s">
+        <v>77</v>
+      </c>
+      <c r="C329" t="s">
+        <v>78</v>
+      </c>
+      <c r="D329" t="s">
+        <v>2</v>
+      </c>
+      <c r="E329" t="s">
+        <v>1</v>
+      </c>
+      <c r="F329">
+        <v>66.53</v>
+      </c>
+      <c r="G329">
+        <v>64.680000000000007</v>
+      </c>
+      <c r="H329">
+        <v>68.37</v>
+      </c>
+    </row>
+    <row r="330" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A330" t="s">
+        <v>85</v>
+      </c>
+      <c r="B330" t="s">
+        <v>81</v>
+      </c>
+      <c r="C330" t="s">
+        <v>82</v>
+      </c>
+      <c r="D330" t="s">
+        <v>0</v>
+      </c>
+      <c r="E330" t="s">
+        <v>1</v>
+      </c>
+      <c r="F330">
+        <v>61.56</v>
+      </c>
+      <c r="G330">
+        <v>59.78</v>
+      </c>
+      <c r="H330">
+        <v>63.34</v>
+      </c>
+    </row>
+    <row r="331" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A331" t="s">
+        <v>85</v>
+      </c>
+      <c r="B331" t="s">
+        <v>81</v>
+      </c>
+      <c r="C331" t="s">
+        <v>82</v>
+      </c>
+      <c r="D331" t="s">
+        <v>2</v>
+      </c>
+      <c r="E331" t="s">
+        <v>1</v>
+      </c>
+      <c r="F331">
+        <v>61.27</v>
+      </c>
+      <c r="G331">
+        <v>59.07</v>
+      </c>
+      <c r="H331">
+        <v>63.46</v>
+      </c>
+    </row>
+    <row r="332" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A332" t="s">
+        <v>85</v>
+      </c>
+      <c r="B332" t="s">
+        <v>83</v>
+      </c>
+      <c r="C332" t="s">
+        <v>84</v>
+      </c>
+      <c r="D332" t="s">
+        <v>0</v>
+      </c>
+      <c r="E332" t="s">
+        <v>1</v>
+      </c>
+      <c r="F332">
+        <v>66.319999999999993</v>
+      </c>
+      <c r="G332">
+        <v>64.540000000000006</v>
+      </c>
+      <c r="H332">
+        <v>68.099999999999994</v>
+      </c>
+    </row>
+    <row r="333" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A333" t="s">
+        <v>85</v>
+      </c>
+      <c r="B333" t="s">
+        <v>83</v>
+      </c>
+      <c r="C333" t="s">
+        <v>84</v>
+      </c>
+      <c r="D333" t="s">
+        <v>2</v>
+      </c>
+      <c r="E333" t="s">
+        <v>1</v>
+      </c>
+      <c r="F333">
+        <v>63.66</v>
+      </c>
+      <c r="G333">
+        <v>61.49</v>
+      </c>
+      <c r="H333">
+        <v>65.84</v>
+      </c>
+    </row>
+    <row r="334" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A334" t="s">
+        <v>85</v>
+      </c>
+      <c r="B334" t="s">
+        <v>86</v>
+      </c>
+      <c r="C334" t="s">
+        <v>80</v>
+      </c>
+      <c r="D334" t="s">
+        <v>0</v>
+      </c>
+      <c r="E334" t="s">
+        <v>1</v>
+      </c>
+      <c r="F334">
+        <v>54.59</v>
+      </c>
+      <c r="G334">
+        <v>52.73</v>
+      </c>
+      <c r="H334">
+        <v>56.45</v>
+      </c>
+    </row>
+    <row r="335" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A335" t="s">
+        <v>85</v>
+      </c>
+      <c r="B335" t="s">
+        <v>86</v>
+      </c>
+      <c r="C335" t="s">
+        <v>80</v>
+      </c>
+      <c r="D335" t="s">
+        <v>2</v>
+      </c>
+      <c r="E335" t="s">
+        <v>1</v>
+      </c>
+      <c r="F335">
+        <v>57.59</v>
+      </c>
+      <c r="G335">
+        <v>55.74</v>
+      </c>
+      <c r="H335">
+        <v>59.44</v>
+      </c>
+    </row>
+    <row r="336" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A336" t="s">
+        <v>85</v>
+      </c>
+      <c r="B336" t="s">
+        <v>87</v>
+      </c>
+      <c r="C336" t="s">
+        <v>76</v>
+      </c>
+      <c r="D336" t="s">
+        <v>0</v>
+      </c>
+      <c r="E336" t="s">
+        <v>1</v>
+      </c>
+      <c r="F336">
+        <v>58.67</v>
+      </c>
+      <c r="G336">
+        <v>56.87</v>
+      </c>
+      <c r="H336">
+        <v>60.46</v>
+      </c>
+    </row>
+    <row r="337" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A337" t="s">
+        <v>85</v>
+      </c>
+      <c r="B337" t="s">
+        <v>87</v>
+      </c>
+      <c r="C337" t="s">
+        <v>76</v>
+      </c>
+      <c r="D337" t="s">
+        <v>2</v>
+      </c>
+      <c r="E337" t="s">
+        <v>1</v>
+      </c>
+      <c r="F337">
+        <v>57.77</v>
+      </c>
+      <c r="G337">
+        <v>55.75</v>
+      </c>
+      <c r="H337">
+        <v>59.79</v>
+      </c>
+    </row>
+    <row r="338" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A338" t="s">
+        <v>85</v>
+      </c>
+      <c r="B338" t="s">
+        <v>3</v>
+      </c>
+      <c r="C338" t="s">
+        <v>4</v>
+      </c>
+      <c r="D338" t="s">
+        <v>2</v>
+      </c>
+      <c r="E338" t="s">
+        <v>1</v>
+      </c>
+      <c r="F338">
+        <v>61.94</v>
+      </c>
+      <c r="G338">
+        <v>61.48</v>
+      </c>
+      <c r="H338">
+        <v>62.4</v>
+      </c>
+    </row>
+    <row r="339" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A339" t="s">
+        <v>85</v>
+      </c>
+      <c r="B339" t="s">
+        <v>3</v>
+      </c>
+      <c r="C339" t="s">
+        <v>4</v>
+      </c>
+      <c r="D339" t="s">
+        <v>0</v>
+      </c>
+      <c r="E339" t="s">
+        <v>1</v>
+      </c>
+      <c r="F339">
+        <v>61.68</v>
+      </c>
+      <c r="G339">
+        <v>61.26</v>
+      </c>
+      <c r="H339">
+        <v>62.09</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState ref="A2:H273">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H273">
     <sortCondition ref="C2:C273"/>
     <sortCondition ref="D2:D273"/>
     <sortCondition ref="A2:A273"/>
@@ -7765,21 +9485,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TrackerID xmlns="e73541d3-5dbc-467b-ad85-92b29e93bc53">685</TrackerID>
     <MoveTo xmlns="2541d45d-41ad-4814-bf67-1422fc7ee58e" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -7920,6 +9640,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1D3EA677-7C4B-4418-9CD0-DA2D17E4A64C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2400BD1B-07FA-4CC2-BD11-B1CD3AC52BA6}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -7932,14 +9660,6 @@
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="2541d45d-41ad-4814-bf67-1422fc7ee58e"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1D3EA677-7C4B-4418-9CD0-DA2D17E4A64C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>